<commit_message>
IC data fra FCT
</commit_message>
<xml_diff>
--- a/data/ICR/ICR_2.xlsx
+++ b/data/ICR/ICR_2.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="598" documentId="8_{8690CADE-2337-47CA-9C98-F2B8AB9E403E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2954E2C3-9FAD-4F99-A4BB-80522CA7E99C}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{03AA78C0-9DD9-4B29-899A-916598C0D743}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{03AA78C0-9DD9-4B29-899A-916598C0D743}"/>
   </bookViews>
   <sheets>
     <sheet name="Cl" sheetId="3" r:id="rId1"/>
@@ -4875,8 +4875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01258D7A-B7F0-4A2F-9E78-30E55431F638}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15749,8 +15749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF89738-146E-48A6-B2D5-0665A64B54DD}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>